<commit_message>
ya se incluyeron varias columnas en DATOS y ya se esta calculando LABEL
</commit_message>
<xml_diff>
--- a/data/periodosRegulares.xlsx
+++ b/data/periodosRegulares.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaimereinoso/DESARROLLO/UAOPiloto/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EC7B203-2613-BD45-999B-A71B319D7BFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE0AC36B-D448-2D4B-8F2E-7FFFA9E4987A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12820" yWindow="7980" windowWidth="28040" windowHeight="17440" xr2:uid="{80B6AC6C-9F2E-C646-BD3C-08E74D641AEF}"/>
   </bookViews>
@@ -36,12 +36,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>periodo</t>
   </si>
   <si>
     <t>orden</t>
+  </si>
+  <si>
+    <t>fecha_inicio</t>
+  </si>
+  <si>
+    <t>fecha_final</t>
   </si>
 </sst>
 </file>
@@ -77,12 +83,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,116 +404,194 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{664E0F50-22D1-894E-91F1-B84A19F49F23}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>201801</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" s="3">
+        <v>43101</v>
+      </c>
+      <c r="D2" s="3">
+        <v>43281</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>201803</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" s="3">
+        <v>43282</v>
+      </c>
+      <c r="D3" s="3">
+        <v>43465</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>201901</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" s="3">
+        <v>43466</v>
+      </c>
+      <c r="D4" s="3">
+        <v>43646</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>201903</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5" s="3">
+        <v>43647</v>
+      </c>
+      <c r="D5" s="3">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>202001</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6" s="3">
+        <v>43831</v>
+      </c>
+      <c r="D6" s="3">
+        <v>44012</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>202003</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7" s="3">
+        <v>44013</v>
+      </c>
+      <c r="D7" s="3">
+        <v>44196</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>202101</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8" s="3">
+        <v>44197</v>
+      </c>
+      <c r="D8" s="3">
+        <v>44377</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>202103</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9" s="3">
+        <v>44378</v>
+      </c>
+      <c r="D9" s="3">
+        <v>44561</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>202201</v>
       </c>
       <c r="B10">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10" s="3">
+        <v>44562</v>
+      </c>
+      <c r="D10" s="3">
+        <v>44742</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>202203</v>
       </c>
       <c r="B11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11" s="3">
+        <v>44743</v>
+      </c>
+      <c r="D11" s="3">
+        <v>44926</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>202301</v>
       </c>
       <c r="B12">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12" s="3">
+        <v>44927</v>
+      </c>
+      <c r="D12" s="3">
+        <v>45107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>202303</v>
       </c>
       <c r="B13">
         <v>12</v>
+      </c>
+      <c r="C13" s="3">
+        <v>45108</v>
+      </c>
+      <c r="D13" s="3">
+        <v>45291</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ya se terminó DATOS y se esta instalando sklearn e imbalanced-learn para proceder con el primer intento
</commit_message>
<xml_diff>
--- a/data/periodosRegulares.xlsx
+++ b/data/periodosRegulares.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaimereinoso/DESARROLLO/UAOPiloto/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE0AC36B-D448-2D4B-8F2E-7FFFA9E4987A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E124DAE-496F-2B47-A5B3-14049171F83B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12820" yWindow="7980" windowWidth="28040" windowHeight="17440" xr2:uid="{80B6AC6C-9F2E-C646-BD3C-08E74D641AEF}"/>
+    <workbookView xWindow="14980" yWindow="7960" windowWidth="28040" windowHeight="17440" xr2:uid="{80B6AC6C-9F2E-C646-BD3C-08E74D641AEF}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -404,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{664E0F50-22D1-894E-91F1-B84A19F49F23}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -427,170 +427,296 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>201801</v>
+      <c r="A2">
+        <v>201303</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" s="3">
-        <v>43101</v>
+        <v>41456</v>
       </c>
       <c r="D2" s="3">
-        <v>43281</v>
+        <v>41639</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>201803</v>
+        <v>201401</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" s="3">
-        <v>43282</v>
+        <v>41640</v>
       </c>
       <c r="D3" s="3">
-        <v>43465</v>
+        <v>41820</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>201901</v>
+        <v>201403</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" s="3">
-        <v>43466</v>
+        <v>41821</v>
       </c>
       <c r="D4" s="3">
-        <v>43646</v>
+        <v>42004</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>201903</v>
+        <v>201501</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" s="3">
-        <v>43647</v>
+        <v>42005</v>
       </c>
       <c r="D5" s="3">
-        <v>43830</v>
+        <v>42185</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>202001</v>
+        <v>201503</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6" s="3">
-        <v>43831</v>
+        <v>42186</v>
       </c>
       <c r="D6" s="3">
-        <v>44012</v>
+        <v>42369</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>202003</v>
+        <v>201601</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
       <c r="C7" s="3">
-        <v>44013</v>
+        <v>42370</v>
       </c>
       <c r="D7" s="3">
-        <v>44196</v>
+        <v>42551</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>202101</v>
+        <v>201603</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
       <c r="C8" s="3">
-        <v>44197</v>
+        <v>42552</v>
       </c>
       <c r="D8" s="3">
-        <v>44377</v>
+        <v>42735</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>202103</v>
+        <v>201701</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
       <c r="C9" s="3">
-        <v>44378</v>
+        <v>42736</v>
       </c>
       <c r="D9" s="3">
-        <v>44561</v>
+        <v>42916</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>202201</v>
+        <v>201703</v>
       </c>
       <c r="B10">
         <v>9</v>
       </c>
       <c r="C10" s="3">
-        <v>44562</v>
+        <v>42917</v>
       </c>
       <c r="D10" s="3">
-        <v>44742</v>
+        <v>43100</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>202203</v>
+      <c r="A11" s="1">
+        <v>201801</v>
       </c>
       <c r="B11">
         <v>10</v>
       </c>
       <c r="C11" s="3">
-        <v>44743</v>
+        <v>43101</v>
       </c>
       <c r="D11" s="3">
-        <v>44926</v>
+        <v>43281</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>202301</v>
+        <v>201803</v>
       </c>
       <c r="B12">
         <v>11</v>
       </c>
       <c r="C12" s="3">
-        <v>44927</v>
+        <v>43282</v>
       </c>
       <c r="D12" s="3">
-        <v>45107</v>
+        <v>43465</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>202303</v>
+        <v>201901</v>
       </c>
       <c r="B13">
         <v>12</v>
       </c>
       <c r="C13" s="3">
+        <v>43466</v>
+      </c>
+      <c r="D13" s="3">
+        <v>43646</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>201903</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14" s="3">
+        <v>43647</v>
+      </c>
+      <c r="D14" s="3">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>202001</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15" s="3">
+        <v>43831</v>
+      </c>
+      <c r="D15" s="3">
+        <v>44012</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>202003</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16" s="3">
+        <v>44013</v>
+      </c>
+      <c r="D16" s="3">
+        <v>44196</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>202101</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17" s="3">
+        <v>44197</v>
+      </c>
+      <c r="D17" s="3">
+        <v>44377</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>202103</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18" s="3">
+        <v>44378</v>
+      </c>
+      <c r="D18" s="3">
+        <v>44561</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>202201</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19" s="3">
+        <v>44562</v>
+      </c>
+      <c r="D19" s="3">
+        <v>44742</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>202203</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20" s="3">
+        <v>44743</v>
+      </c>
+      <c r="D20" s="3">
+        <v>44926</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>202301</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21" s="3">
+        <v>44927</v>
+      </c>
+      <c r="D21" s="3">
+        <v>45107</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>202303</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22" s="3">
         <v>45108</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D22" s="3">
         <v>45291</v>
       </c>
     </row>

</xml_diff>